<commit_message>
Micro benchmark timing after enabling term build caching
</commit_message>
<xml_diff>
--- a/org.metaborg.lang.tiger.example/microbenchmarks/timings.xlsx
+++ b/org.metaborg.lang.tiger.example/microbenchmarks/timings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="32740" windowHeight="20540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="32740" windowHeight="20540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="queens-looped" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <t>JDK</t>
   </si>
   <si>
-    <t>Stable Trees</t>
+    <t>Cached Term Builds</t>
   </si>
 </sst>
 </file>
@@ -483,6 +483,261 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'queens-looped'!$E$1:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames Directed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'queens-looped'!$E$4:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2910.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2389.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2334.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2344.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2419.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3337.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2289.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2369.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2255.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2393.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2289.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2279.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2335.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2280.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2310.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2315.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2287.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2454.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2293.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2226.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2415.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'queens-looped'!$F$1:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'queens-looped'!$F$4:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'queens-looped'!$G$1:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Environments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'queens-looped'!$G$4:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1535.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1135.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1273.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>961.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>970.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>945.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>994.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>998.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>994.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>973.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>961.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>959.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>967.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>958.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>954.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>978.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1011.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>981.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>962.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>963.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>964.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -492,11 +747,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1699958816"/>
-        <c:axId val="-1699963296"/>
+        <c:axId val="-1694825120"/>
+        <c:axId val="-1681950400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1699958816"/>
+        <c:axId val="-1694825120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -538,7 +793,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1699963296"/>
+        <c:crossAx val="-1681950400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -546,7 +801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1699963296"/>
+        <c:axId val="-1681950400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -596,7 +851,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1699958816"/>
+        <c:crossAx val="-1694825120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1046,6 +1301,261 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>branching!$E$1:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames Directed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>branching!$E$4:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>293.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>126.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>38.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>branching!$F$1:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>branching!$F$4:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>branching!$G$1:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Environments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>branching!$G$4:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>196.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1055,11 +1565,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1699950928"/>
-        <c:axId val="-1694598976"/>
+        <c:axId val="-1695783968"/>
+        <c:axId val="-1697581936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1699950928"/>
+        <c:axId val="-1695783968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1101,7 +1611,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1694598976"/>
+        <c:crossAx val="-1697581936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1109,7 +1619,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1694598976"/>
+        <c:axId val="-1697581936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1159,7 +1669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1699950928"/>
+        <c:crossAx val="-1695783968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1609,6 +2119,261 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'var-local'!$E$1:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames Directed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'var-local'!$E$4:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>171.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>106.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'var-local'!$F$1:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'var-local'!$F$4:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'var-local'!$G$1:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Environments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'var-local'!$G$4:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>137.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>18.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1618,11 +2383,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1695306512"/>
-        <c:axId val="-1695308464"/>
+        <c:axId val="-1681214576"/>
+        <c:axId val="-1684391872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1695306512"/>
+        <c:axId val="-1681214576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1664,7 +2429,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1695308464"/>
+        <c:crossAx val="-1684391872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1672,7 +2437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1695308464"/>
+        <c:axId val="-1684391872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1692,7 +2457,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1723,7 +2487,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1695306512"/>
+        <c:crossAx val="-1681214576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2173,6 +2937,261 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'var-parent'!$E$1:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames Directed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'var-parent'!$E$4:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>276.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>112.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>73.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>108.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'var-parent'!$F$1:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'var-parent'!$F$4:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'var-parent'!$G$1:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Environments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'var-parent'!$G$4:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>135.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2182,11 +3201,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1685119184"/>
-        <c:axId val="-1685093584"/>
+        <c:axId val="-1683097168"/>
+        <c:axId val="-1695464992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1685119184"/>
+        <c:axId val="-1683097168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2228,7 +3247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1685093584"/>
+        <c:crossAx val="-1695464992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2236,7 +3255,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1685093584"/>
+        <c:axId val="-1695464992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2286,7 +3305,762 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1685119184"/>
+        <c:crossAx val="-1683097168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'while-loop'!$B$1:$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Baseline DynSem</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames Directed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'while-loop'!$B$4:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1900.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>664.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>573.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>570.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>685.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>499.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>501.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>610.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>506.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>608.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>629.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>501.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>501.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>573.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>526.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>578.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1617.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>490.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>489.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'while-loop'!$C$1:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Baseline DynSem</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'while-loop'!$C$4:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'while-loop'!$D$1:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Baseline DynSem</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Environments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'while-loop'!$D$4:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>655.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>373.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>192.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>228.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>249.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>207.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>301.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>165.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>235.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>191.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>243.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>254.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>165.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>169.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>160.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'while-loop'!$E$1:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames Directed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'while-loop'!$E$4:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1706.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>776.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>575.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>508.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>573.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>484.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>498.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>702.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>495.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>570.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>476.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>529.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>678.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>508.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>488.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>565.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>494.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>509.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>747.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>480.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>495.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'while-loop'!$F$1:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'while-loop'!$F$4:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'while-loop'!$G$1:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cached Term Builds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Environments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'while-loop'!$G$4:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>737.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>417.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>223.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>252.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>275.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>182.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>245.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>308.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>227.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>245.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>298.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>182.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>164.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>248.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>281.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>252.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>202.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>185.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>162.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>163.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1685962784"/>
+        <c:axId val="-1697164528"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1685962784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1697164528"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1697164528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1685962784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2527,6 +4301,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4591,20 +6405,571 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4626,59 +6991,24 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>901700</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4700,16 +7030,51 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4997,7 +7362,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G3"/>
+      <selection activeCell="G3" sqref="B1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5065,6 +7430,12 @@
       <c r="D4" s="2">
         <v>1702</v>
       </c>
+      <c r="E4" s="2">
+        <v>2910</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1535</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -5079,6 +7450,12 @@
       <c r="D5" s="2">
         <v>1135</v>
       </c>
+      <c r="E5" s="2">
+        <v>2389</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1135</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -5093,6 +7470,12 @@
       <c r="D6" s="2">
         <v>1304</v>
       </c>
+      <c r="E6" s="2">
+        <v>2334</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1273</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -5107,6 +7490,12 @@
       <c r="D7" s="2">
         <v>995</v>
       </c>
+      <c r="E7" s="2">
+        <v>2344</v>
+      </c>
+      <c r="G7" s="2">
+        <v>961</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -5121,6 +7510,12 @@
       <c r="D8" s="2">
         <v>935</v>
       </c>
+      <c r="E8" s="2">
+        <v>2419</v>
+      </c>
+      <c r="G8" s="2">
+        <v>970</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -5135,6 +7530,12 @@
       <c r="D9" s="2">
         <v>946</v>
       </c>
+      <c r="E9" s="2">
+        <v>3337</v>
+      </c>
+      <c r="G9" s="2">
+        <v>945</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -5149,6 +7550,12 @@
       <c r="D10" s="2">
         <v>968</v>
       </c>
+      <c r="E10" s="2">
+        <v>2289</v>
+      </c>
+      <c r="G10" s="2">
+        <v>994</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -5163,6 +7570,12 @@
       <c r="D11" s="2">
         <v>950</v>
       </c>
+      <c r="E11" s="2">
+        <v>2369</v>
+      </c>
+      <c r="G11" s="2">
+        <v>998</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -5177,6 +7590,12 @@
       <c r="D12" s="2">
         <v>950</v>
       </c>
+      <c r="E12" s="2">
+        <v>2255</v>
+      </c>
+      <c r="G12" s="2">
+        <v>994</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -5191,6 +7610,12 @@
       <c r="D13" s="2">
         <v>1034</v>
       </c>
+      <c r="E13" s="2">
+        <v>2393</v>
+      </c>
+      <c r="G13" s="2">
+        <v>973</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -5205,6 +7630,12 @@
       <c r="D14" s="2">
         <v>977</v>
       </c>
+      <c r="E14" s="2">
+        <v>2289</v>
+      </c>
+      <c r="G14" s="2">
+        <v>961</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -5219,6 +7650,12 @@
       <c r="D15" s="2">
         <v>969</v>
       </c>
+      <c r="E15" s="2">
+        <v>2279</v>
+      </c>
+      <c r="G15" s="2">
+        <v>959</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -5233,8 +7670,14 @@
       <c r="D16" s="2">
         <v>965</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2">
+        <v>2335</v>
+      </c>
+      <c r="G16" s="2">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
@@ -5247,8 +7690,14 @@
       <c r="D17" s="2">
         <v>943</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2">
+        <v>2280</v>
+      </c>
+      <c r="G17" s="2">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
@@ -5261,8 +7710,14 @@
       <c r="D18" s="2">
         <v>949</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="2">
+        <v>2310</v>
+      </c>
+      <c r="G18" s="2">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
@@ -5275,8 +7730,14 @@
       <c r="D19" s="2">
         <v>928</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="2">
+        <v>2315</v>
+      </c>
+      <c r="G19" s="2">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
@@ -5289,8 +7750,14 @@
       <c r="D20" s="2">
         <v>934</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="2">
+        <v>2287</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
@@ -5303,8 +7770,14 @@
       <c r="D21" s="2">
         <v>971</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2">
+        <v>2454</v>
+      </c>
+      <c r="G21" s="2">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
@@ -5317,8 +7790,14 @@
       <c r="D22" s="2">
         <v>983</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="2">
+        <v>2293</v>
+      </c>
+      <c r="G22" s="2">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
@@ -5331,8 +7810,14 @@
       <c r="D23" s="2">
         <v>979</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="2">
+        <v>2226</v>
+      </c>
+      <c r="G23" s="2">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
@@ -5343,6 +7828,12 @@
         <v>2156</v>
       </c>
       <c r="D24" s="2">
+        <v>964</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2415</v>
+      </c>
+      <c r="G24" s="2">
         <v>964</v>
       </c>
     </row>
@@ -5361,8 +7852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5429,6 +7920,12 @@
       <c r="D4" s="2">
         <v>195</v>
       </c>
+      <c r="E4" s="2">
+        <v>293</v>
+      </c>
+      <c r="G4" s="2">
+        <v>196</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
@@ -5440,6 +7937,12 @@
       <c r="D5" s="2">
         <v>111</v>
       </c>
+      <c r="E5" s="2">
+        <v>126</v>
+      </c>
+      <c r="G5" s="2">
+        <v>99</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
@@ -5451,6 +7954,12 @@
       <c r="D6" s="2">
         <v>58</v>
       </c>
+      <c r="E6" s="2">
+        <v>69</v>
+      </c>
+      <c r="G6" s="2">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
@@ -5462,6 +7971,12 @@
       <c r="D7" s="2">
         <v>69</v>
       </c>
+      <c r="E7" s="2">
+        <v>89</v>
+      </c>
+      <c r="G7" s="2">
+        <v>51</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
@@ -5473,6 +7988,12 @@
       <c r="D8" s="2">
         <v>57</v>
       </c>
+      <c r="E8" s="2">
+        <v>76</v>
+      </c>
+      <c r="G8" s="2">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
@@ -5484,6 +8005,12 @@
       <c r="D9" s="2">
         <v>31</v>
       </c>
+      <c r="E9" s="2">
+        <v>86</v>
+      </c>
+      <c r="G9" s="2">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
@@ -5495,6 +8022,12 @@
       <c r="D10" s="2">
         <v>39</v>
       </c>
+      <c r="E10" s="2">
+        <v>62</v>
+      </c>
+      <c r="G10" s="2">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
@@ -5506,6 +8039,12 @@
       <c r="D11" s="2">
         <v>29</v>
       </c>
+      <c r="E11" s="2">
+        <v>59</v>
+      </c>
+      <c r="G11" s="2">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
@@ -5517,6 +8056,12 @@
       <c r="D12" s="2">
         <v>20</v>
       </c>
+      <c r="E12" s="2">
+        <v>60</v>
+      </c>
+      <c r="G12" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
@@ -5528,6 +8073,12 @@
       <c r="D13" s="2">
         <v>41</v>
       </c>
+      <c r="E13" s="2">
+        <v>53</v>
+      </c>
+      <c r="G13" s="2">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
@@ -5539,6 +8090,12 @@
       <c r="D14" s="2">
         <v>39</v>
       </c>
+      <c r="E14" s="2">
+        <v>35</v>
+      </c>
+      <c r="G14" s="2">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
@@ -5550,6 +8107,12 @@
       <c r="D15" s="2">
         <v>33</v>
       </c>
+      <c r="E15" s="2">
+        <v>31</v>
+      </c>
+      <c r="G15" s="2">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
@@ -5561,8 +8124,14 @@
       <c r="D16" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2">
+        <v>34</v>
+      </c>
+      <c r="G16" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>35</v>
       </c>
@@ -5572,8 +8141,14 @@
       <c r="D17" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2">
+        <v>29</v>
+      </c>
+      <c r="G17" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>38</v>
       </c>
@@ -5583,8 +8158,14 @@
       <c r="D18" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="2">
+        <v>38</v>
+      </c>
+      <c r="G18" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>35</v>
       </c>
@@ -5594,8 +8175,14 @@
       <c r="D19" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="2">
+        <v>32</v>
+      </c>
+      <c r="G19" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>30</v>
       </c>
@@ -5605,8 +8192,14 @@
       <c r="D20" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="2">
+        <v>41</v>
+      </c>
+      <c r="G20" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>31</v>
       </c>
@@ -5616,8 +8209,14 @@
       <c r="D21" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2">
+        <v>34</v>
+      </c>
+      <c r="G21" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>31</v>
       </c>
@@ -5627,8 +8226,14 @@
       <c r="D22" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="2">
+        <v>33</v>
+      </c>
+      <c r="G22" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>31</v>
       </c>
@@ -5638,8 +8243,14 @@
       <c r="D23" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="2">
+        <v>31</v>
+      </c>
+      <c r="G23" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>28</v>
       </c>
@@ -5648,6 +8259,12 @@
       </c>
       <c r="D24" s="2">
         <v>32</v>
+      </c>
+      <c r="E24" s="2">
+        <v>38</v>
+      </c>
+      <c r="G24" s="2">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -5666,7 +8283,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G4" sqref="G4:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5735,6 +8352,12 @@
       <c r="D4" s="2">
         <v>103</v>
       </c>
+      <c r="E4" s="2">
+        <v>171</v>
+      </c>
+      <c r="G4" s="2">
+        <v>137</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
@@ -5746,6 +8369,12 @@
       <c r="D5" s="2">
         <v>78</v>
       </c>
+      <c r="E5" s="2">
+        <v>106</v>
+      </c>
+      <c r="G5" s="2">
+        <v>74</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
@@ -5757,6 +8386,12 @@
       <c r="D6" s="2">
         <v>42</v>
       </c>
+      <c r="E6" s="2">
+        <v>50</v>
+      </c>
+      <c r="G6" s="2">
+        <v>54</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
@@ -5768,6 +8403,12 @@
       <c r="D7" s="2">
         <v>59</v>
       </c>
+      <c r="E7" s="2">
+        <v>58</v>
+      </c>
+      <c r="G7" s="2">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
@@ -5779,6 +8420,12 @@
       <c r="D8" s="2">
         <v>25</v>
       </c>
+      <c r="E8" s="2">
+        <v>37</v>
+      </c>
+      <c r="G8" s="2">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
@@ -5790,6 +8437,12 @@
       <c r="D9" s="2">
         <v>25</v>
       </c>
+      <c r="E9" s="2">
+        <v>40</v>
+      </c>
+      <c r="G9" s="2">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
@@ -5801,6 +8454,12 @@
       <c r="D10" s="2">
         <v>40</v>
       </c>
+      <c r="E10" s="2">
+        <v>35</v>
+      </c>
+      <c r="G10" s="2">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
@@ -5812,6 +8471,12 @@
       <c r="D11" s="2">
         <v>18</v>
       </c>
+      <c r="E11" s="2">
+        <v>32</v>
+      </c>
+      <c r="G11" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
@@ -5823,6 +8488,12 @@
       <c r="D12" s="2">
         <v>17</v>
       </c>
+      <c r="E12" s="2">
+        <v>37</v>
+      </c>
+      <c r="G12" s="2">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
@@ -5834,6 +8505,12 @@
       <c r="D13" s="2">
         <v>28</v>
       </c>
+      <c r="E13" s="2">
+        <v>43</v>
+      </c>
+      <c r="G13" s="2">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
@@ -5845,6 +8522,12 @@
       <c r="D14" s="2">
         <v>27</v>
       </c>
+      <c r="E14" s="2">
+        <v>40</v>
+      </c>
+      <c r="G14" s="2">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
@@ -5856,6 +8539,12 @@
       <c r="D15" s="2">
         <v>14</v>
       </c>
+      <c r="E15" s="2">
+        <v>48</v>
+      </c>
+      <c r="G15" s="2">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
@@ -5867,8 +8556,14 @@
       <c r="D16" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2">
+        <v>37</v>
+      </c>
+      <c r="G16" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>34</v>
       </c>
@@ -5878,8 +8573,14 @@
       <c r="D17" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2">
+        <v>44</v>
+      </c>
+      <c r="G17" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>36</v>
       </c>
@@ -5889,8 +8590,14 @@
       <c r="D18" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="2">
+        <v>38</v>
+      </c>
+      <c r="G18" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>39</v>
       </c>
@@ -5900,8 +8607,14 @@
       <c r="D19" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="2">
+        <v>44</v>
+      </c>
+      <c r="G19" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>31</v>
       </c>
@@ -5911,8 +8624,14 @@
       <c r="D20" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="2">
+        <v>30</v>
+      </c>
+      <c r="G20" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>28</v>
       </c>
@@ -5922,8 +8641,14 @@
       <c r="D21" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2">
+        <v>36</v>
+      </c>
+      <c r="G21" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>48</v>
       </c>
@@ -5933,8 +8658,14 @@
       <c r="D22" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="2">
+        <v>28</v>
+      </c>
+      <c r="G22" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>49</v>
       </c>
@@ -5944,8 +8675,14 @@
       <c r="D23" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="2">
+        <v>26</v>
+      </c>
+      <c r="G23" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>27</v>
       </c>
@@ -5954,6 +8691,12 @@
       </c>
       <c r="D24" s="2">
         <v>13</v>
+      </c>
+      <c r="E24" s="2">
+        <v>39</v>
+      </c>
+      <c r="G24" s="2">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -5972,7 +8715,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G3"/>
+      <selection activeCell="G4" sqref="G4:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6041,6 +8784,12 @@
       <c r="D4" s="2">
         <v>137</v>
       </c>
+      <c r="E4" s="2">
+        <v>276</v>
+      </c>
+      <c r="G4" s="2">
+        <v>135</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
@@ -6052,6 +8801,12 @@
       <c r="D5" s="2">
         <v>75</v>
       </c>
+      <c r="E5" s="2">
+        <v>112</v>
+      </c>
+      <c r="G5" s="2">
+        <v>79</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
@@ -6063,6 +8818,12 @@
       <c r="D6" s="2">
         <v>50</v>
       </c>
+      <c r="E6" s="2">
+        <v>96</v>
+      </c>
+      <c r="G6" s="2">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
@@ -6074,6 +8835,12 @@
       <c r="D7" s="2">
         <v>37</v>
       </c>
+      <c r="E7" s="2">
+        <v>70</v>
+      </c>
+      <c r="G7" s="2">
+        <v>44</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
@@ -6085,6 +8852,12 @@
       <c r="D8" s="2">
         <v>45</v>
       </c>
+      <c r="E8" s="2">
+        <v>74</v>
+      </c>
+      <c r="G8" s="2">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
@@ -6096,6 +8869,12 @@
       <c r="D9" s="2">
         <v>25</v>
       </c>
+      <c r="E9" s="2">
+        <v>77</v>
+      </c>
+      <c r="G9" s="2">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
@@ -6107,6 +8886,12 @@
       <c r="D10" s="2">
         <v>25</v>
       </c>
+      <c r="E10" s="2">
+        <v>71</v>
+      </c>
+      <c r="G10" s="2">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
@@ -6118,6 +8903,12 @@
       <c r="D11" s="2">
         <v>39</v>
       </c>
+      <c r="E11" s="2">
+        <v>73</v>
+      </c>
+      <c r="G11" s="2">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
@@ -6129,6 +8920,12 @@
       <c r="D12" s="2">
         <v>21</v>
       </c>
+      <c r="E12" s="2">
+        <v>67</v>
+      </c>
+      <c r="G12" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
@@ -6140,6 +8937,12 @@
       <c r="D13" s="2">
         <v>17</v>
       </c>
+      <c r="E13" s="2">
+        <v>59</v>
+      </c>
+      <c r="G13" s="2">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
@@ -6151,6 +8954,12 @@
       <c r="D14" s="2">
         <v>28</v>
       </c>
+      <c r="E14" s="2">
+        <v>51</v>
+      </c>
+      <c r="G14" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
@@ -6162,6 +8971,12 @@
       <c r="D15" s="2">
         <v>19</v>
       </c>
+      <c r="E15" s="2">
+        <v>51</v>
+      </c>
+      <c r="G15" s="2">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
@@ -6173,8 +8988,14 @@
       <c r="D16" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2">
+        <v>56</v>
+      </c>
+      <c r="G16" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>31</v>
       </c>
@@ -6184,8 +9005,14 @@
       <c r="D17" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2">
+        <v>108</v>
+      </c>
+      <c r="G17" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>39</v>
       </c>
@@ -6195,8 +9022,14 @@
       <c r="D18" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="2">
+        <v>31</v>
+      </c>
+      <c r="G18" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>27</v>
       </c>
@@ -6206,8 +9039,14 @@
       <c r="D19" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="2">
+        <v>37</v>
+      </c>
+      <c r="G19" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>34</v>
       </c>
@@ -6217,8 +9056,14 @@
       <c r="D20" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="2">
+        <v>41</v>
+      </c>
+      <c r="G20" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>38</v>
       </c>
@@ -6228,8 +9073,14 @@
       <c r="D21" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2">
+        <v>32</v>
+      </c>
+      <c r="G21" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>28</v>
       </c>
@@ -6239,8 +9090,14 @@
       <c r="D22" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="2">
+        <v>31</v>
+      </c>
+      <c r="G22" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>29</v>
       </c>
@@ -6250,8 +9107,14 @@
       <c r="D23" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="2">
+        <v>30</v>
+      </c>
+      <c r="G23" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>36</v>
       </c>
@@ -6260,6 +9123,12 @@
       </c>
       <c r="D24" s="2">
         <v>19</v>
+      </c>
+      <c r="E24" s="2">
+        <v>32</v>
+      </c>
+      <c r="G24" s="2">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -6277,11 +9146,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
@@ -6335,6 +9207,12 @@
       <c r="D4" s="2">
         <v>655</v>
       </c>
+      <c r="E4" s="2">
+        <v>1706</v>
+      </c>
+      <c r="G4" s="2">
+        <v>737</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
@@ -6343,6 +9221,12 @@
       <c r="D5" s="2">
         <v>373</v>
       </c>
+      <c r="E5" s="2">
+        <v>776</v>
+      </c>
+      <c r="G5" s="2">
+        <v>417</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
@@ -6351,6 +9235,12 @@
       <c r="D6" s="2">
         <v>192</v>
       </c>
+      <c r="E6" s="2">
+        <v>575</v>
+      </c>
+      <c r="G6" s="2">
+        <v>223</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
@@ -6359,6 +9249,12 @@
       <c r="D7" s="2">
         <v>228</v>
       </c>
+      <c r="E7" s="2">
+        <v>508</v>
+      </c>
+      <c r="G7" s="2">
+        <v>252</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
@@ -6367,6 +9263,12 @@
       <c r="D8" s="2">
         <v>249</v>
       </c>
+      <c r="E8" s="2">
+        <v>573</v>
+      </c>
+      <c r="G8" s="2">
+        <v>275</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
@@ -6375,6 +9277,12 @@
       <c r="D9" s="2">
         <v>156</v>
       </c>
+      <c r="E9" s="2">
+        <v>484</v>
+      </c>
+      <c r="G9" s="2">
+        <v>182</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
@@ -6383,6 +9291,12 @@
       <c r="D10" s="2">
         <v>207</v>
       </c>
+      <c r="E10" s="2">
+        <v>498</v>
+      </c>
+      <c r="G10" s="2">
+        <v>245</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
@@ -6391,6 +9305,12 @@
       <c r="D11" s="2">
         <v>301</v>
       </c>
+      <c r="E11" s="2">
+        <v>702</v>
+      </c>
+      <c r="G11" s="2">
+        <v>308</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
@@ -6399,6 +9319,12 @@
       <c r="D12" s="2">
         <v>165</v>
       </c>
+      <c r="E12" s="2">
+        <v>495</v>
+      </c>
+      <c r="G12" s="2">
+        <v>227</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
@@ -6407,6 +9333,12 @@
       <c r="D13" s="2">
         <v>160</v>
       </c>
+      <c r="E13" s="2">
+        <v>570</v>
+      </c>
+      <c r="G13" s="2">
+        <v>245</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
@@ -6415,6 +9347,12 @@
       <c r="D14" s="2">
         <v>235</v>
       </c>
+      <c r="E14" s="2">
+        <v>476</v>
+      </c>
+      <c r="G14" s="2">
+        <v>298</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
@@ -6423,6 +9361,12 @@
       <c r="D15" s="2">
         <v>151</v>
       </c>
+      <c r="E15" s="2">
+        <v>529</v>
+      </c>
+      <c r="G15" s="2">
+        <v>182</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
@@ -6431,69 +9375,123 @@
       <c r="D16" s="2">
         <v>154</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2">
+        <v>678</v>
+      </c>
+      <c r="G16" s="2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>501</v>
       </c>
       <c r="D17" s="2">
         <v>191</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2">
+        <v>508</v>
+      </c>
+      <c r="G17" s="2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>573</v>
       </c>
       <c r="D18" s="2">
         <v>243</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="2">
+        <v>488</v>
+      </c>
+      <c r="G18" s="2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>526</v>
       </c>
       <c r="D19" s="2">
         <v>254</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="2">
+        <v>565</v>
+      </c>
+      <c r="G19" s="2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>512</v>
       </c>
       <c r="D20" s="2">
         <v>161</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="2">
+        <v>494</v>
+      </c>
+      <c r="G20" s="2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>578</v>
       </c>
       <c r="D21" s="2">
         <v>165</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2">
+        <v>509</v>
+      </c>
+      <c r="G21" s="2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>1617</v>
       </c>
       <c r="D22" s="2">
         <v>169</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="2">
+        <v>747</v>
+      </c>
+      <c r="G22" s="2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>490</v>
       </c>
       <c r="D23" s="2">
         <v>150</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="2">
+        <v>480</v>
+      </c>
+      <c r="G23" s="2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>489</v>
       </c>
       <c r="D24" s="2">
         <v>160</v>
+      </c>
+      <c r="E24" s="2">
+        <v>495</v>
+      </c>
+      <c r="G24" s="2">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -6503,5 +9501,6 @@
     <mergeCell ref="E2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Timings after enabling pushing down term builds
</commit_message>
<xml_diff>
--- a/org.metaborg.lang.tiger.example/microbenchmarks/timings.xlsx
+++ b/org.metaborg.lang.tiger.example/microbenchmarks/timings.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="9">
   <si>
     <t>Iteration</t>
   </si>
@@ -56,12 +56,15 @@
   <si>
     <t>No caching wrappers</t>
   </si>
+  <si>
+    <t>Pushdown termbuild</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -74,6 +77,29 @@
       <color theme="1"/>
       <name val="Monaco"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,17 +119,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -938,6 +976,267 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'queens-looped'!$K$1:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames Directed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'queens-looped'!$K$4:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2359.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1692.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1718.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1674.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1767.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1717.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1679.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1688.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1624.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1678.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1583.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1711.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1580.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1732.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1628.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1559.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1730.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1636.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1541.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1642.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1691.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'queens-looped'!$L$1:$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'queens-looped'!$L$4:$L$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'queens-looped'!$M$1:$M$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Environments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'queens-looped'!$M$4:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1135.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>861.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1038.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>723.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>843.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>911.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>720.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>692.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>735.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>686.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>686.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>693.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>742.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>696.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>755.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>705.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>719.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>709.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>697.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -947,11 +1246,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1648310912"/>
-        <c:axId val="-1650937520"/>
+        <c:axId val="-1645696208"/>
+        <c:axId val="-1684619872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1648310912"/>
+        <c:axId val="-1645696208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -993,7 +1292,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1650937520"/>
+        <c:crossAx val="-1684619872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1001,7 +1300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1650937520"/>
+        <c:axId val="-1684619872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1051,7 +1350,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1648310912"/>
+        <c:crossAx val="-1645696208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1954,6 +2253,267 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>branching!$K$1:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames Directed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>branching!$K$4:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>139.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>135.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>branching!$L$1:$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>branching!$L$4:$L$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>branching!$M$1:$M$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Environments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>branching!$M$4:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1963,11 +2523,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1695428720"/>
-        <c:axId val="-1684639312"/>
+        <c:axId val="-1652027376"/>
+        <c:axId val="-1685998416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1695428720"/>
+        <c:axId val="-1652027376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2009,7 +2569,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1684639312"/>
+        <c:crossAx val="-1685998416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2017,7 +2577,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1684639312"/>
+        <c:axId val="-1685998416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2067,7 +2627,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1695428720"/>
+        <c:crossAx val="-1652027376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2970,6 +3530,267 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'var-local'!$K$1:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames Directed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'var-local'!$K$4:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>108.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'var-local'!$L$1:$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'var-local'!$L$4:$L$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'var-local'!$M$1:$M$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Environments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'var-local'!$M$4:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2979,11 +3800,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1685893712"/>
-        <c:axId val="-1647874016"/>
+        <c:axId val="-1651725632"/>
+        <c:axId val="-1651723856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1685893712"/>
+        <c:axId val="-1651725632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3025,7 +3846,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1647874016"/>
+        <c:crossAx val="-1651723856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3033,7 +3854,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1647874016"/>
+        <c:axId val="-1651723856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3083,7 +3904,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1685893712"/>
+        <c:crossAx val="-1651725632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3986,6 +4807,267 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'var-parent'!$K$1:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames Directed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'var-parent'!$K$4:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'var-parent'!$L$1:$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'var-parent'!$L$4:$L$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'var-parent'!$M$1:$M$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Environments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'var-parent'!$M$4:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>92.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -3995,11 +5077,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1696950288"/>
-        <c:axId val="-1647456544"/>
+        <c:axId val="-1682948768"/>
+        <c:axId val="-1694611568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1696950288"/>
+        <c:axId val="-1682948768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4041,7 +5123,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1647456544"/>
+        <c:crossAx val="-1694611568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4049,7 +5131,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1647456544"/>
+        <c:axId val="-1694611568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4099,7 +5181,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1696950288"/>
+        <c:crossAx val="-1682948768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4939,6 +6021,267 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'while-loop'!$K$1:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames Directed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'while-loop'!$K$4:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2016.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>571.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>594.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>373.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>394.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>363.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>576.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>355.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>354.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>399.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>352.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>417.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>574.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>355.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>342.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>364.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>937.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>358.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>342.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>391.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>592.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'while-loop'!$L$1:$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'while-loop'!$L$4:$L$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'while-loop'!$M$1:$M$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JDK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pushdown termbuild</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Environments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'while-loop'!$M$4:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>534.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>197.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>236.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>112.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>279.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>113.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>113.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>195.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>107.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>108.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>119.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>202.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>195.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>183.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>105.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>109.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>110.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>118.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -4948,11 +6291,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1696043536"/>
-        <c:axId val="-1698175936"/>
+        <c:axId val="-1697771248"/>
+        <c:axId val="-1644527184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1696043536"/>
+        <c:axId val="-1697771248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4994,7 +6337,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1698175936"/>
+        <c:crossAx val="-1644527184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5002,7 +6345,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1698175936"/>
+        <c:axId val="-1644527184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5052,7 +6395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1696043536"/>
+        <c:crossAx val="-1697771248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7918,19 +9261,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:colOff>800100</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="7" name="Chart 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7952,20 +9295,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7987,20 +9330,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8022,20 +9365,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8057,20 +9400,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8351,19 +9694,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="16.5" customWidth="1"/>
+    <col min="11" max="11" width="22.5" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -8375,8 +9720,11 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8392,8 +9740,13 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -8424,8 +9777,17 @@
       <c r="J3" t="s">
         <v>4</v>
       </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -8447,8 +9809,14 @@
       <c r="J4" s="2">
         <v>1610</v>
       </c>
+      <c r="K4" s="2">
+        <v>2359</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1135</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -8470,8 +9838,14 @@
       <c r="J5" s="2">
         <v>1157</v>
       </c>
+      <c r="K5" s="2">
+        <v>1692</v>
+      </c>
+      <c r="M5" s="2">
+        <v>861</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -8493,8 +9867,14 @@
       <c r="J6" s="2">
         <v>1297</v>
       </c>
+      <c r="K6" s="2">
+        <v>1718</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1038</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -8516,8 +9896,14 @@
       <c r="J7" s="2">
         <v>1010</v>
       </c>
+      <c r="K7" s="2">
+        <v>1674</v>
+      </c>
+      <c r="M7" s="2">
+        <v>723</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -8539,8 +9925,14 @@
       <c r="J8" s="2">
         <v>1021</v>
       </c>
+      <c r="K8" s="2">
+        <v>1767</v>
+      </c>
+      <c r="M8" s="2">
+        <v>843</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -8562,8 +9954,14 @@
       <c r="J9" s="2">
         <v>1057</v>
       </c>
+      <c r="K9" s="2">
+        <v>1717</v>
+      </c>
+      <c r="M9" s="2">
+        <v>911</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -8585,8 +9983,14 @@
       <c r="J10" s="2">
         <v>1003</v>
       </c>
+      <c r="K10" s="2">
+        <v>1679</v>
+      </c>
+      <c r="M10" s="2">
+        <v>720</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -8608,8 +10012,14 @@
       <c r="J11" s="2">
         <v>996</v>
       </c>
+      <c r="K11" s="2">
+        <v>1688</v>
+      </c>
+      <c r="M11" s="2">
+        <v>692</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -8631,8 +10041,14 @@
       <c r="J12" s="2">
         <v>1003</v>
       </c>
+      <c r="K12" s="2">
+        <v>1624</v>
+      </c>
+      <c r="M12" s="2">
+        <v>735</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -8654,8 +10070,14 @@
       <c r="J13" s="2">
         <v>1013</v>
       </c>
+      <c r="K13" s="2">
+        <v>1678</v>
+      </c>
+      <c r="M13" s="2">
+        <v>700</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -8677,8 +10099,14 @@
       <c r="J14" s="2">
         <v>986</v>
       </c>
+      <c r="K14" s="2">
+        <v>1583</v>
+      </c>
+      <c r="M14" s="2">
+        <v>686</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -8700,8 +10128,14 @@
       <c r="J15" s="2">
         <v>992</v>
       </c>
+      <c r="K15" s="2">
+        <v>1711</v>
+      </c>
+      <c r="M15" s="2">
+        <v>686</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
@@ -8723,8 +10157,14 @@
       <c r="J16" s="2">
         <v>980</v>
       </c>
+      <c r="K16" s="2">
+        <v>1580</v>
+      </c>
+      <c r="M16" s="2">
+        <v>700</v>
+      </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
@@ -8746,8 +10186,14 @@
       <c r="J17" s="2">
         <v>989</v>
       </c>
+      <c r="K17" s="2">
+        <v>1732</v>
+      </c>
+      <c r="M17" s="2">
+        <v>693</v>
+      </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
@@ -8769,8 +10215,14 @@
       <c r="J18" s="2">
         <v>1002</v>
       </c>
+      <c r="K18" s="2">
+        <v>1628</v>
+      </c>
+      <c r="M18" s="2">
+        <v>742</v>
+      </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
@@ -8792,8 +10244,14 @@
       <c r="J19" s="2">
         <v>1023</v>
       </c>
+      <c r="K19" s="2">
+        <v>1559</v>
+      </c>
+      <c r="M19" s="2">
+        <v>696</v>
+      </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
@@ -8815,8 +10273,14 @@
       <c r="J20" s="2">
         <v>967</v>
       </c>
+      <c r="K20" s="2">
+        <v>1730</v>
+      </c>
+      <c r="M20" s="2">
+        <v>755</v>
+      </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
@@ -8838,8 +10302,14 @@
       <c r="J21" s="2">
         <v>984</v>
       </c>
+      <c r="K21" s="2">
+        <v>1636</v>
+      </c>
+      <c r="M21" s="2">
+        <v>705</v>
+      </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
@@ -8861,8 +10331,14 @@
       <c r="J22" s="2">
         <v>965</v>
       </c>
+      <c r="K22" s="2">
+        <v>1541</v>
+      </c>
+      <c r="M22" s="2">
+        <v>719</v>
+      </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
@@ -8884,8 +10360,14 @@
       <c r="J23" s="2">
         <v>960</v>
       </c>
+      <c r="K23" s="2">
+        <v>1642</v>
+      </c>
+      <c r="M23" s="2">
+        <v>709</v>
+      </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
@@ -8907,12 +10389,19 @@
       <c r="J24" s="2">
         <v>990</v>
       </c>
+      <c r="K24" s="2">
+        <v>1691</v>
+      </c>
+      <c r="M24" s="2">
+        <v>697</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B1:J1"/>
     <mergeCell ref="H2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8922,10 +10411,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J3"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8939,69 +10428,88 @@
     <col min="10" max="10" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="K3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>322</v>
       </c>
@@ -9020,8 +10528,14 @@
       <c r="J4" s="2">
         <v>209</v>
       </c>
+      <c r="K4" s="2">
+        <v>139</v>
+      </c>
+      <c r="M4" s="2">
+        <v>148</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>84</v>
       </c>
@@ -9040,8 +10554,14 @@
       <c r="J5" s="2">
         <v>88</v>
       </c>
+      <c r="K5" s="2">
+        <v>89</v>
+      </c>
+      <c r="M5" s="2">
+        <v>43</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>74</v>
       </c>
@@ -9060,8 +10580,14 @@
       <c r="J6" s="2">
         <v>75</v>
       </c>
+      <c r="K6" s="2">
+        <v>94</v>
+      </c>
+      <c r="M6" s="2">
+        <v>49</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>76</v>
       </c>
@@ -9080,8 +10606,14 @@
       <c r="J7" s="2">
         <v>79</v>
       </c>
+      <c r="K7" s="2">
+        <v>67</v>
+      </c>
+      <c r="M7" s="2">
+        <v>30</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>73</v>
       </c>
@@ -9100,8 +10632,14 @@
       <c r="J8" s="2">
         <v>85</v>
       </c>
+      <c r="K8" s="2">
+        <v>63</v>
+      </c>
+      <c r="M8" s="2">
+        <v>40</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>73</v>
       </c>
@@ -9120,8 +10658,14 @@
       <c r="J9" s="2">
         <v>36</v>
       </c>
+      <c r="K9" s="2">
+        <v>135</v>
+      </c>
+      <c r="M9" s="2">
+        <v>34</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>56</v>
       </c>
@@ -9140,8 +10684,14 @@
       <c r="J10" s="2">
         <v>39</v>
       </c>
+      <c r="K10" s="2">
+        <v>28</v>
+      </c>
+      <c r="M10" s="2">
+        <v>25</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>71</v>
       </c>
@@ -9160,8 +10710,14 @@
       <c r="J11" s="2">
         <v>48</v>
       </c>
+      <c r="K11" s="2">
+        <v>26</v>
+      </c>
+      <c r="M11" s="2">
+        <v>25</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>60</v>
       </c>
@@ -9180,8 +10736,14 @@
       <c r="J12" s="2">
         <v>27</v>
       </c>
+      <c r="K12" s="2">
+        <v>42</v>
+      </c>
+      <c r="M12" s="2">
+        <v>32</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>94</v>
       </c>
@@ -9200,8 +10762,14 @@
       <c r="J13" s="2">
         <v>33</v>
       </c>
+      <c r="K13" s="2">
+        <v>23</v>
+      </c>
+      <c r="M13" s="2">
+        <v>25</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>33</v>
       </c>
@@ -9220,8 +10788,14 @@
       <c r="J14" s="2">
         <v>43</v>
       </c>
+      <c r="K14" s="2">
+        <v>28</v>
+      </c>
+      <c r="M14" s="2">
+        <v>29</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>33</v>
       </c>
@@ -9240,8 +10814,14 @@
       <c r="J15" s="2">
         <v>38</v>
       </c>
+      <c r="K15" s="2">
+        <v>30</v>
+      </c>
+      <c r="M15" s="2">
+        <v>26</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>30</v>
       </c>
@@ -9260,8 +10840,14 @@
       <c r="J16" s="2">
         <v>31</v>
       </c>
+      <c r="K16" s="2">
+        <v>25</v>
+      </c>
+      <c r="M16" s="2">
+        <v>21</v>
+      </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>35</v>
       </c>
@@ -9280,8 +10866,14 @@
       <c r="J17" s="2">
         <v>26</v>
       </c>
+      <c r="K17" s="2">
+        <v>19</v>
+      </c>
+      <c r="M17" s="2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>38</v>
       </c>
@@ -9300,8 +10892,14 @@
       <c r="J18" s="2">
         <v>36</v>
       </c>
+      <c r="K18" s="2">
+        <v>22</v>
+      </c>
+      <c r="M18" s="2">
+        <v>24</v>
+      </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>35</v>
       </c>
@@ -9320,8 +10918,14 @@
       <c r="J19" s="2">
         <v>20</v>
       </c>
+      <c r="K19" s="2">
+        <v>22</v>
+      </c>
+      <c r="M19" s="2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>30</v>
       </c>
@@ -9340,8 +10944,14 @@
       <c r="J20" s="2">
         <v>35</v>
       </c>
+      <c r="K20" s="2">
+        <v>20</v>
+      </c>
+      <c r="M20" s="2">
+        <v>28</v>
+      </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>31</v>
       </c>
@@ -9360,8 +10970,14 @@
       <c r="J21" s="2">
         <v>20</v>
       </c>
+      <c r="K21" s="2">
+        <v>32</v>
+      </c>
+      <c r="M21" s="2">
+        <v>15</v>
+      </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>31</v>
       </c>
@@ -9380,8 +10996,14 @@
       <c r="J22" s="2">
         <v>28</v>
       </c>
+      <c r="K22" s="2">
+        <v>26</v>
+      </c>
+      <c r="M22" s="2">
+        <v>17</v>
+      </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>31</v>
       </c>
@@ -9400,8 +11022,14 @@
       <c r="J23" s="2">
         <v>21</v>
       </c>
+      <c r="K23" s="2">
+        <v>19</v>
+      </c>
+      <c r="M23" s="2">
+        <v>12</v>
+      </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>28</v>
       </c>
@@ -9420,13 +11048,20 @@
       <c r="J24" s="2">
         <v>19</v>
       </c>
+      <c r="K24" s="2">
+        <v>26</v>
+      </c>
+      <c r="M24" s="2">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9435,10 +11070,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B3" sqref="B1:J1048576"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9453,69 +11088,88 @@
     <col min="10" max="10" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="K3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>170</v>
       </c>
@@ -9534,8 +11188,14 @@
       <c r="J4" s="2">
         <v>103</v>
       </c>
+      <c r="K4" s="2">
+        <v>108</v>
+      </c>
+      <c r="M4" s="2">
+        <v>63</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>124</v>
       </c>
@@ -9554,8 +11214,14 @@
       <c r="J5" s="2">
         <v>58</v>
       </c>
+      <c r="K5" s="2">
+        <v>54</v>
+      </c>
+      <c r="M5" s="2">
+        <v>32</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>49</v>
       </c>
@@ -9574,8 +11240,14 @@
       <c r="J6" s="2">
         <v>48</v>
       </c>
+      <c r="K6" s="2">
+        <v>54</v>
+      </c>
+      <c r="M6" s="2">
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>69</v>
       </c>
@@ -9594,8 +11266,14 @@
       <c r="J7" s="2">
         <v>44</v>
       </c>
+      <c r="K7" s="2">
+        <v>38</v>
+      </c>
+      <c r="M7" s="2">
+        <v>38</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>43</v>
       </c>
@@ -9614,8 +11292,14 @@
       <c r="J8" s="2">
         <v>31</v>
       </c>
+      <c r="K8" s="2">
+        <v>49</v>
+      </c>
+      <c r="M8" s="2">
+        <v>19</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>57</v>
       </c>
@@ -9634,8 +11318,14 @@
       <c r="J9" s="2">
         <v>31</v>
       </c>
+      <c r="K9" s="2">
+        <v>37</v>
+      </c>
+      <c r="M9" s="2">
+        <v>27</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>31</v>
       </c>
@@ -9654,8 +11344,14 @@
       <c r="J10" s="2">
         <v>43</v>
       </c>
+      <c r="K10" s="2">
+        <v>47</v>
+      </c>
+      <c r="M10" s="2">
+        <v>18</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>40</v>
       </c>
@@ -9674,8 +11370,14 @@
       <c r="J11" s="2">
         <v>23</v>
       </c>
+      <c r="K11" s="2">
+        <v>36</v>
+      </c>
+      <c r="M11" s="2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>41</v>
       </c>
@@ -9694,8 +11396,14 @@
       <c r="J12" s="2">
         <v>20</v>
       </c>
+      <c r="K12" s="2">
+        <v>39</v>
+      </c>
+      <c r="M12" s="2">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>48</v>
       </c>
@@ -9714,8 +11422,14 @@
       <c r="J13" s="2">
         <v>29</v>
       </c>
+      <c r="K13" s="2">
+        <v>44</v>
+      </c>
+      <c r="M13" s="2">
+        <v>24</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>49</v>
       </c>
@@ -9734,8 +11448,14 @@
       <c r="J14" s="2">
         <v>33</v>
       </c>
+      <c r="K14" s="2">
+        <v>51</v>
+      </c>
+      <c r="M14" s="2">
+        <v>14</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>56</v>
       </c>
@@ -9754,8 +11474,14 @@
       <c r="J15" s="2">
         <v>18</v>
       </c>
+      <c r="K15" s="2">
+        <v>36</v>
+      </c>
+      <c r="M15" s="2">
+        <v>11</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>32</v>
       </c>
@@ -9774,8 +11500,14 @@
       <c r="J16" s="2">
         <v>15</v>
       </c>
+      <c r="K16" s="2">
+        <v>53</v>
+      </c>
+      <c r="M16" s="2">
+        <v>16</v>
+      </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>34</v>
       </c>
@@ -9794,8 +11526,14 @@
       <c r="J17" s="2">
         <v>13</v>
       </c>
+      <c r="K17" s="2">
+        <v>30</v>
+      </c>
+      <c r="M17" s="2">
+        <v>19</v>
+      </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>36</v>
       </c>
@@ -9814,8 +11552,14 @@
       <c r="J18" s="2">
         <v>17</v>
       </c>
+      <c r="K18" s="2">
+        <v>29</v>
+      </c>
+      <c r="M18" s="2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>39</v>
       </c>
@@ -9834,8 +11578,14 @@
       <c r="J19" s="2">
         <v>20</v>
       </c>
+      <c r="K19" s="2">
+        <v>35</v>
+      </c>
+      <c r="M19" s="2">
+        <v>12</v>
+      </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>31</v>
       </c>
@@ -9854,8 +11604,14 @@
       <c r="J20" s="2">
         <v>10</v>
       </c>
+      <c r="K20" s="2">
+        <v>34</v>
+      </c>
+      <c r="M20" s="2">
+        <v>19</v>
+      </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>28</v>
       </c>
@@ -9874,8 +11630,14 @@
       <c r="J21" s="2">
         <v>11</v>
       </c>
+      <c r="K21" s="2">
+        <v>33</v>
+      </c>
+      <c r="M21" s="2">
+        <v>16</v>
+      </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>48</v>
       </c>
@@ -9894,8 +11656,14 @@
       <c r="J22" s="2">
         <v>11</v>
       </c>
+      <c r="K22" s="2">
+        <v>34</v>
+      </c>
+      <c r="M22" s="2">
+        <v>26</v>
+      </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>49</v>
       </c>
@@ -9914,8 +11682,14 @@
       <c r="J23" s="2">
         <v>17</v>
       </c>
+      <c r="K23" s="2">
+        <v>31</v>
+      </c>
+      <c r="M23" s="2">
+        <v>18</v>
+      </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>27</v>
       </c>
@@ -9934,13 +11708,20 @@
       <c r="J24" s="2">
         <v>18</v>
       </c>
+      <c r="K24" s="2">
+        <v>32</v>
+      </c>
+      <c r="M24" s="2">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9949,10 +11730,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B1:J1048576"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9966,69 +11747,88 @@
     <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="K3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>279</v>
       </c>
@@ -10047,8 +11847,14 @@
       <c r="J4" s="2">
         <v>122</v>
       </c>
+      <c r="K4" s="2">
+        <v>161</v>
+      </c>
+      <c r="M4" s="2">
+        <v>92</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>130</v>
       </c>
@@ -10067,8 +11873,14 @@
       <c r="J5" s="2">
         <v>71</v>
       </c>
+      <c r="K5" s="2">
+        <v>95</v>
+      </c>
+      <c r="M5" s="2">
+        <v>39</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>111</v>
       </c>
@@ -10087,8 +11899,14 @@
       <c r="J6" s="2">
         <v>61</v>
       </c>
+      <c r="K6" s="2">
+        <v>81</v>
+      </c>
+      <c r="M6" s="2">
+        <v>32</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>67</v>
       </c>
@@ -10107,8 +11925,14 @@
       <c r="J7" s="2">
         <v>40</v>
       </c>
+      <c r="K7" s="2">
+        <v>77</v>
+      </c>
+      <c r="M7" s="2">
+        <v>36</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>77</v>
       </c>
@@ -10127,8 +11951,14 @@
       <c r="J8" s="2">
         <v>48</v>
       </c>
+      <c r="K8" s="2">
+        <v>67</v>
+      </c>
+      <c r="M8" s="2">
+        <v>23</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>78</v>
       </c>
@@ -10147,8 +11977,14 @@
       <c r="J9" s="2">
         <v>24</v>
       </c>
+      <c r="K9" s="2">
+        <v>66</v>
+      </c>
+      <c r="M9" s="2">
+        <v>32</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>74</v>
       </c>
@@ -10167,8 +12003,14 @@
       <c r="J10" s="2">
         <v>23</v>
       </c>
+      <c r="K10" s="2">
+        <v>91</v>
+      </c>
+      <c r="M10" s="2">
+        <v>18</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>45</v>
       </c>
@@ -10187,8 +12029,14 @@
       <c r="J11" s="2">
         <v>33</v>
       </c>
+      <c r="K11" s="2">
+        <v>61</v>
+      </c>
+      <c r="M11" s="2">
+        <v>24</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>61</v>
       </c>
@@ -10207,8 +12055,14 @@
       <c r="J12" s="2">
         <v>21</v>
       </c>
+      <c r="K12" s="2">
+        <v>60</v>
+      </c>
+      <c r="M12" s="2">
+        <v>14</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>96</v>
       </c>
@@ -10227,8 +12081,14 @@
       <c r="J13" s="2">
         <v>21</v>
       </c>
+      <c r="K13" s="2">
+        <v>67</v>
+      </c>
+      <c r="M13" s="2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>44</v>
       </c>
@@ -10247,8 +12107,14 @@
       <c r="J14" s="2">
         <v>41</v>
       </c>
+      <c r="K14" s="2">
+        <v>52</v>
+      </c>
+      <c r="M14" s="2">
+        <v>24</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>60</v>
       </c>
@@ -10267,8 +12133,14 @@
       <c r="J15" s="2">
         <v>19</v>
       </c>
+      <c r="K15" s="2">
+        <v>80</v>
+      </c>
+      <c r="M15" s="2">
+        <v>17</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>99</v>
       </c>
@@ -10287,8 +12159,14 @@
       <c r="J16" s="2">
         <v>20</v>
       </c>
+      <c r="K16" s="2">
+        <v>61</v>
+      </c>
+      <c r="M16" s="2">
+        <v>18</v>
+      </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>31</v>
       </c>
@@ -10307,8 +12185,14 @@
       <c r="J17" s="2">
         <v>19</v>
       </c>
+      <c r="K17" s="2">
+        <v>149</v>
+      </c>
+      <c r="M17" s="2">
+        <v>15</v>
+      </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>39</v>
       </c>
@@ -10327,8 +12211,14 @@
       <c r="J18" s="2">
         <v>25</v>
       </c>
+      <c r="K18" s="2">
+        <v>38</v>
+      </c>
+      <c r="M18" s="2">
+        <v>17</v>
+      </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>27</v>
       </c>
@@ -10347,8 +12237,14 @@
       <c r="J19" s="2">
         <v>18</v>
       </c>
+      <c r="K19" s="2">
+        <v>33</v>
+      </c>
+      <c r="M19" s="2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>34</v>
       </c>
@@ -10367,8 +12263,14 @@
       <c r="J20" s="2">
         <v>13</v>
       </c>
+      <c r="K20" s="2">
+        <v>39</v>
+      </c>
+      <c r="M20" s="2">
+        <v>21</v>
+      </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>38</v>
       </c>
@@ -10387,8 +12289,14 @@
       <c r="J21" s="2">
         <v>20</v>
       </c>
+      <c r="K21" s="2">
+        <v>37</v>
+      </c>
+      <c r="M21" s="2">
+        <v>12</v>
+      </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>28</v>
       </c>
@@ -10407,8 +12315,14 @@
       <c r="J22" s="2">
         <v>17</v>
       </c>
+      <c r="K22" s="2">
+        <v>44</v>
+      </c>
+      <c r="M22" s="2">
+        <v>18</v>
+      </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>29</v>
       </c>
@@ -10427,8 +12341,14 @@
       <c r="J23" s="2">
         <v>24</v>
       </c>
+      <c r="K23" s="2">
+        <v>40</v>
+      </c>
+      <c r="M23" s="2">
+        <v>16</v>
+      </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>36</v>
       </c>
@@ -10447,13 +12367,20 @@
       <c r="J24" s="2">
         <v>14</v>
       </c>
+      <c r="K24" s="2">
+        <v>22</v>
+      </c>
+      <c r="M24" s="2">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B1:J1"/>
     <mergeCell ref="H2:J2"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10462,10 +12389,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="K4" sqref="K4:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10473,69 +12400,88 @@
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="K3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>1900</v>
       </c>
@@ -10551,8 +12497,14 @@
       <c r="J4" s="2">
         <v>655</v>
       </c>
+      <c r="K4" s="2">
+        <v>2016</v>
+      </c>
+      <c r="M4" s="2">
+        <v>534</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>664</v>
       </c>
@@ -10568,8 +12520,14 @@
       <c r="J5" s="2">
         <v>403</v>
       </c>
+      <c r="K5" s="2">
+        <v>571</v>
+      </c>
+      <c r="M5" s="2">
+        <v>360</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>573</v>
       </c>
@@ -10585,8 +12543,14 @@
       <c r="J6" s="2">
         <v>188</v>
       </c>
+      <c r="K6" s="2">
+        <v>594</v>
+      </c>
+      <c r="M6" s="2">
+        <v>142</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>570</v>
       </c>
@@ -10602,8 +12566,14 @@
       <c r="J7" s="2">
         <v>238</v>
       </c>
+      <c r="K7" s="2">
+        <v>373</v>
+      </c>
+      <c r="M7" s="2">
+        <v>197</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>512</v>
       </c>
@@ -10619,8 +12589,14 @@
       <c r="J8" s="2">
         <v>274</v>
       </c>
+      <c r="K8" s="2">
+        <v>394</v>
+      </c>
+      <c r="M8" s="2">
+        <v>236</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>685</v>
       </c>
@@ -10636,8 +12612,14 @@
       <c r="J9" s="2">
         <v>151</v>
       </c>
+      <c r="K9" s="2">
+        <v>363</v>
+      </c>
+      <c r="M9" s="2">
+        <v>112</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>499</v>
       </c>
@@ -10653,8 +12635,14 @@
       <c r="J10" s="2">
         <v>217</v>
       </c>
+      <c r="K10" s="2">
+        <v>576</v>
+      </c>
+      <c r="M10" s="2">
+        <v>146</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>501</v>
       </c>
@@ -10670,8 +12658,14 @@
       <c r="J11" s="2">
         <v>300</v>
       </c>
+      <c r="K11" s="2">
+        <v>355</v>
+      </c>
+      <c r="M11" s="2">
+        <v>279</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>610</v>
       </c>
@@ -10687,8 +12681,14 @@
       <c r="J12" s="2">
         <v>173</v>
       </c>
+      <c r="K12" s="2">
+        <v>354</v>
+      </c>
+      <c r="M12" s="2">
+        <v>113</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>506</v>
       </c>
@@ -10704,8 +12704,14 @@
       <c r="J13" s="2">
         <v>158</v>
       </c>
+      <c r="K13" s="2">
+        <v>399</v>
+      </c>
+      <c r="M13" s="2">
+        <v>113</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>608</v>
       </c>
@@ -10721,8 +12727,14 @@
       <c r="J14" s="2">
         <v>221</v>
       </c>
+      <c r="K14" s="2">
+        <v>352</v>
+      </c>
+      <c r="M14" s="2">
+        <v>195</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>629</v>
       </c>
@@ -10738,8 +12750,14 @@
       <c r="J15" s="2">
         <v>153</v>
       </c>
+      <c r="K15" s="2">
+        <v>417</v>
+      </c>
+      <c r="M15" s="2">
+        <v>107</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>501</v>
       </c>
@@ -10755,8 +12773,14 @@
       <c r="J16" s="2">
         <v>158</v>
       </c>
+      <c r="K16" s="2">
+        <v>574</v>
+      </c>
+      <c r="M16" s="2">
+        <v>108</v>
+      </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>501</v>
       </c>
@@ -10772,8 +12796,14 @@
       <c r="J17" s="2">
         <v>199</v>
       </c>
+      <c r="K17" s="2">
+        <v>355</v>
+      </c>
+      <c r="M17" s="2">
+        <v>119</v>
+      </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>573</v>
       </c>
@@ -10789,8 +12819,14 @@
       <c r="J18" s="2">
         <v>248</v>
       </c>
+      <c r="K18" s="2">
+        <v>342</v>
+      </c>
+      <c r="M18" s="2">
+        <v>202</v>
+      </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>526</v>
       </c>
@@ -10806,8 +12842,14 @@
       <c r="J19" s="2">
         <v>268</v>
       </c>
+      <c r="K19" s="2">
+        <v>364</v>
+      </c>
+      <c r="M19" s="2">
+        <v>195</v>
+      </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>512</v>
       </c>
@@ -10823,8 +12865,14 @@
       <c r="J20" s="2">
         <v>177</v>
       </c>
+      <c r="K20" s="2">
+        <v>937</v>
+      </c>
+      <c r="M20" s="2">
+        <v>183</v>
+      </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>578</v>
       </c>
@@ -10840,8 +12888,14 @@
       <c r="J21" s="2">
         <v>165</v>
       </c>
+      <c r="K21" s="2">
+        <v>358</v>
+      </c>
+      <c r="M21" s="2">
+        <v>105</v>
+      </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>1617</v>
       </c>
@@ -10857,8 +12911,14 @@
       <c r="J22" s="2">
         <v>163</v>
       </c>
+      <c r="K22" s="2">
+        <v>342</v>
+      </c>
+      <c r="M22" s="2">
+        <v>109</v>
+      </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>490</v>
       </c>
@@ -10874,8 +12934,14 @@
       <c r="J23" s="2">
         <v>159</v>
       </c>
+      <c r="K23" s="2">
+        <v>391</v>
+      </c>
+      <c r="M23" s="2">
+        <v>110</v>
+      </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>489</v>
       </c>
@@ -10891,13 +12957,20 @@
       <c r="J24" s="2">
         <v>161</v>
       </c>
+      <c r="K24" s="2">
+        <v>592</v>
+      </c>
+      <c r="M24" s="2">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B1:J1"/>
     <mergeCell ref="H2:J2"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Implement sieve of Eratosthenes as benchmark
</commit_message>
<xml_diff>
--- a/org.metaborg.lang.tiger.example/microbenchmarks/timings.xlsx
+++ b/org.metaborg.lang.tiger.example/microbenchmarks/timings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="32740" windowHeight="20540" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="32740" windowHeight="20540" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="queens-looped" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="var-parent" sheetId="4" r:id="rId4"/>
     <sheet name="while-loop" sheetId="5" r:id="rId5"/>
     <sheet name="break-intensive" sheetId="6" r:id="rId6"/>
+    <sheet name="sieve" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="16">
   <si>
     <t>Iteration</t>
   </si>
@@ -64,22 +65,22 @@
     <t xml:space="preserve">Frames </t>
   </si>
   <si>
-    <t>Frames EXP-lib</t>
-  </si>
-  <si>
     <t>bed0099f8 -- Extendible Explication</t>
   </si>
   <si>
     <t>da6342b83 -- Native EXC support</t>
   </si>
   <si>
-    <t>Frames EXP-nat</t>
-  </si>
-  <si>
     <t>Frames EXC-lib</t>
   </si>
   <si>
     <t>Frames EXC-nat</t>
+  </si>
+  <si>
+    <t>5353df0622f -- RuleChains</t>
+  </si>
+  <si>
+    <t>5353df0622f -- FatChain</t>
   </si>
 </sst>
 </file>
@@ -166,7 +167,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -175,6 +176,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -791,6 +793,112 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'queens-looped'!$O$1:$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>GraalVM-0.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5353df0622f -- RuleChains</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames EXC-nat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'queens-looped'!$O$4:$O$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>12075.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>267.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>112.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>116.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>117.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>123.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>182.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>115.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>124.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>114.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>115.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>135.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>217.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -800,11 +908,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1698808272"/>
-        <c:axId val="-1699290400"/>
+        <c:axId val="-1608618416"/>
+        <c:axId val="-1680217936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1698808272"/>
+        <c:axId val="-1608618416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,7 +954,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1699290400"/>
+        <c:crossAx val="-1680217936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -854,10 +962,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1699290400"/>
+        <c:axId val="-1680217936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="500.0"/>
+          <c:max val="300.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -875,6 +983,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -905,7 +1014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1698808272"/>
+        <c:crossAx val="-1608618416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1934,7 +2043,7 @@
                   <c:v>bed0099f8 -- Extendible Explication</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Frames EXP-lib</c:v>
+                  <c:v>Frames EXC-lib</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2146,7 +2255,7 @@
                   <c:v>da6342b83 -- Native EXC support</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Frames EXP-nat</c:v>
+                  <c:v>Frames EXC-nat</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2252,7 +2361,7 @@
                   <c:v>da6342b83 -- Native EXC support</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Frames EXP-lib</c:v>
+                  <c:v>Frames EXC-lib</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2710,7 +2819,7 @@
                   <c:v>bed0099f8 -- Extendible Explication</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Frames EXP-lib</c:v>
+                  <c:v>Frames EXC-lib</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2922,7 +3031,7 @@
                   <c:v>da6342b83 -- Native EXC support</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Frames EXP-nat</c:v>
+                  <c:v>Frames EXC-nat</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3028,7 +3137,7 @@
                   <c:v>da6342b83 -- Native EXC support</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Frames EXP-lib</c:v>
+                  <c:v>Frames EXC-lib</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3486,7 +3595,7 @@
                   <c:v>bed0099f8 -- Extendible Explication</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Frames EXP-lib</c:v>
+                  <c:v>Frames EXC-lib</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3698,7 +3807,7 @@
                   <c:v>da6342b83 -- Native EXC support</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Frames EXP-nat</c:v>
+                  <c:v>Frames EXC-nat</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3804,7 +3913,7 @@
                   <c:v>da6342b83 -- Native EXC support</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Frames EXP-lib</c:v>
+                  <c:v>Frames EXC-lib</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4146,14 +4255,14 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'break-intensive'!$B$1:$B$3</c:f>
+              <c:f>'break-intensive'!$J$1:$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>JDK</c:v>
+                  <c:v>GraalVM-0.32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Baseline DynSem</c:v>
+                  <c:v>0b275500eac -- Indirect Call Node</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Frames </c:v>
@@ -4165,356 +4274,6 @@
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'break-intensive'!$B$4:$B$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'break-intensive'!$C$1:$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>JDK</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Baseline DynSem</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Environments</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'break-intensive'!$C$4:$C$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'break-intensive'!$D$1:$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>JDK</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Cached Term Builds</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Frames </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'break-intensive'!$D$4:$D$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'break-intensive'!$E$1:$E$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>JDK</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Cached Term Builds</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Environments</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'break-intensive'!$E$4:$E$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'break-intensive'!$F$1:$F$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>JDK</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>No caching wrappers</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Frames </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'break-intensive'!$F$4:$F$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'break-intensive'!$G$1:$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>JDK</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>No caching wrappers</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Environments</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'break-intensive'!$G$4:$G$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'break-intensive'!$H$1:$H$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>JDK</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Pushdown termbuild</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Frames </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'break-intensive'!$H$4:$H$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'break-intensive'!$I$1:$I$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>JDK</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Pushdown termbuild</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Environments</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'break-intensive'!$I$4:$I$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'break-intensive'!$J$1:$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>GraalVM-0.32</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0b275500eac -- Indirect Call Node</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Frames </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4535,8 +4294,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>'break-intensive'!$K$1:$K$3</c:f>
@@ -4549,7 +4308,7 @@
                   <c:v>bed0099f8 -- Extendible Explication</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Frames EXP-lib</c:v>
+                  <c:v>Frames EXC-lib</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4557,9 +4316,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4580,8 +4337,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="10"/>
-          <c:order val="10"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>'break-intensive'!$L$1:$L$3</c:f>
@@ -4602,9 +4359,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4625,8 +4380,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="11"/>
-          <c:order val="11"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>'break-intensive'!$M$1:$M$3</c:f>
@@ -4639,7 +4394,7 @@
                   <c:v>da6342b83 -- Native EXC support</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Frames EXP-nat</c:v>
+                  <c:v>Frames EXC-nat</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4647,9 +4402,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4733,8 +4486,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="12"/>
-          <c:order val="12"/>
+          <c:idx val="4"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>'break-intensive'!$N$1:$N$3</c:f>
@@ -4747,7 +4500,7 @@
                   <c:v>da6342b83 -- Native EXC support</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Frames EXP-lib</c:v>
+                  <c:v>Frames EXC-lib</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4755,10 +4508,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4841,6 +4591,112 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'break-intensive'!$O$1:$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>GraalVM-0.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5353df0622f -- RuleChains</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Frames EXC-nat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'break-intensive'!$O$4:$O$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>7691.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1994.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>367.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>206.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>322.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>217.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>224.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>227.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>466.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>217.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>290.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>244.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>224.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>221.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>308.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>470.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>228.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>225.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>233.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>610.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -4850,11 +4706,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2113503760"/>
-        <c:axId val="-1700261664"/>
+        <c:axId val="-1649124224"/>
+        <c:axId val="-1646090368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2113503760"/>
+        <c:axId val="-1649124224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4896,7 +4752,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1700261664"/>
+        <c:crossAx val="-1646090368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4904,10 +4760,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1700261664"/>
+        <c:axId val="-1646090368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="500.0"/>
+          <c:max val="1000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4925,7 +4781,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4956,7 +4811,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2113503760"/>
+        <c:crossAx val="-1649124224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8377,20 +8232,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvPr id="13" name="Chart 12"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8518,15 +8373,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8553,19 +8408,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8846,10 +8701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M5:M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8863,20 +8718,21 @@
     <col min="12" max="12" width="18.5" customWidth="1"/>
     <col min="13" max="13" width="15.33203125" customWidth="1"/>
     <col min="14" max="14" width="22" customWidth="1"/>
+    <col min="15" max="16" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
@@ -8884,82 +8740,95 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="L3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -8999,8 +8868,11 @@
       <c r="N4" s="3">
         <v>8353</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="3">
+        <v>12075</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -9040,8 +8912,11 @@
       <c r="N5" s="3">
         <v>4659</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -9081,8 +8956,11 @@
       <c r="N6" s="3">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" s="3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -9122,8 +9000,11 @@
       <c r="N7" s="3">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -9163,8 +9044,11 @@
       <c r="N8" s="3">
         <v>260</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -9204,8 +9088,11 @@
       <c r="N9" s="3">
         <v>179</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -9245,8 +9132,11 @@
       <c r="N10" s="3">
         <v>133</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -9286,8 +9176,11 @@
       <c r="N11" s="3">
         <v>119</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -9327,8 +9220,11 @@
       <c r="N12" s="3">
         <v>119</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12" s="3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -9368,8 +9264,11 @@
       <c r="N13" s="3">
         <v>128</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13" s="3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -9409,8 +9308,11 @@
       <c r="N14" s="3">
         <v>120</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -9450,8 +9352,11 @@
       <c r="N15" s="3">
         <v>201</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15" s="3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
@@ -9491,8 +9396,11 @@
       <c r="N16" s="3">
         <v>122</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16" s="3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
@@ -9532,8 +9440,11 @@
       <c r="N17" s="3">
         <v>129</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17" s="3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
@@ -9573,8 +9484,11 @@
       <c r="N18" s="3">
         <v>120</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
@@ -9614,8 +9528,11 @@
       <c r="N19" s="3">
         <v>115</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19" s="3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
@@ -9655,8 +9572,11 @@
       <c r="N20" s="3">
         <v>133</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20" s="3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
@@ -9696,8 +9616,11 @@
       <c r="N21" s="3">
         <v>123</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21" s="3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
@@ -9737,8 +9660,11 @@
       <c r="N22" s="3">
         <v>122</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
@@ -9778,8 +9704,11 @@
       <c r="N23" s="3">
         <v>241</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O23" s="3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
@@ -9818,12 +9747,15 @@
       </c>
       <c r="N24" s="3">
         <v>119</v>
+      </c>
+      <c r="O24" s="3">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="J1:O1"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="B1:I1"/>
@@ -9838,10 +9770,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J2" sqref="J1:N1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O24" sqref="O6:O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9860,20 +9792,21 @@
     <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
@@ -9881,82 +9814,89 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="L3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <v>322</v>
       </c>
@@ -9993,8 +9933,11 @@
       <c r="N4" s="3">
         <v>2220</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="3">
+        <v>2528</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>84</v>
       </c>
@@ -10031,8 +9974,11 @@
       <c r="N5" s="3">
         <v>3359</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="3">
+        <v>2810</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>74</v>
       </c>
@@ -10069,8 +10015,11 @@
       <c r="N6" s="3">
         <v>386</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>76</v>
       </c>
@@ -10107,8 +10056,11 @@
       <c r="N7" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <v>73</v>
       </c>
@@ -10145,8 +10097,11 @@
       <c r="N8" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>73</v>
       </c>
@@ -10183,8 +10138,11 @@
       <c r="N9" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>56</v>
       </c>
@@ -10221,8 +10179,11 @@
       <c r="N10" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>71</v>
       </c>
@@ -10259,8 +10220,11 @@
       <c r="N11" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>60</v>
       </c>
@@ -10297,8 +10261,11 @@
       <c r="N12" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>94</v>
       </c>
@@ -10335,8 +10302,11 @@
       <c r="N13" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>33</v>
       </c>
@@ -10373,8 +10343,11 @@
       <c r="N14" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>33</v>
       </c>
@@ -10411,8 +10384,11 @@
       <c r="N15" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>30</v>
       </c>
@@ -10449,8 +10425,11 @@
       <c r="N16" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <v>35</v>
       </c>
@@ -10487,8 +10466,11 @@
       <c r="N17" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O17" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <v>38</v>
       </c>
@@ -10525,8 +10507,11 @@
       <c r="N18" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>35</v>
       </c>
@@ -10563,8 +10548,11 @@
       <c r="N19" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O19" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>30</v>
       </c>
@@ -10601,8 +10589,11 @@
       <c r="N20" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O20" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <v>31</v>
       </c>
@@ -10639,8 +10630,11 @@
       <c r="N21" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O21" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <v>31</v>
       </c>
@@ -10677,8 +10671,11 @@
       <c r="N22" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <v>31</v>
       </c>
@@ -10715,8 +10712,11 @@
       <c r="N23" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O23" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <v>28</v>
       </c>
@@ -10753,11 +10753,14 @@
       <c r="N24" s="3">
         <v>3</v>
       </c>
+      <c r="O24" s="3">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="J1:N1"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="J1:O1"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -10772,10 +10775,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="J2" sqref="J1:N1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9:M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10794,18 +10797,18 @@
     <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
@@ -10813,82 +10816,89 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="L3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <v>170</v>
       </c>
@@ -10925,8 +10935,11 @@
       <c r="N4" s="3">
         <v>207</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>124</v>
       </c>
@@ -10963,8 +10976,11 @@
       <c r="N5" s="3">
         <v>599</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="3">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>49</v>
       </c>
@@ -11001,8 +11017,11 @@
       <c r="N6" s="3">
         <v>2189</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" s="3">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>69</v>
       </c>
@@ -11039,8 +11058,11 @@
       <c r="N7" s="3">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <v>43</v>
       </c>
@@ -11077,8 +11099,11 @@
       <c r="N8" s="3">
         <v>6157</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="3">
+        <v>5002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>57</v>
       </c>
@@ -11115,8 +11140,11 @@
       <c r="N9" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>31</v>
       </c>
@@ -11153,8 +11181,11 @@
       <c r="N10" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>40</v>
       </c>
@@ -11191,8 +11222,11 @@
       <c r="N11" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>41</v>
       </c>
@@ -11229,8 +11263,11 @@
       <c r="N12" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>48</v>
       </c>
@@ -11267,8 +11304,11 @@
       <c r="N13" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>49</v>
       </c>
@@ -11305,8 +11345,11 @@
       <c r="N14" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>56</v>
       </c>
@@ -11343,8 +11386,11 @@
       <c r="N15" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>32</v>
       </c>
@@ -11381,8 +11427,11 @@
       <c r="N16" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <v>34</v>
       </c>
@@ -11419,8 +11468,11 @@
       <c r="N17" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O17" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <v>36</v>
       </c>
@@ -11457,8 +11509,11 @@
       <c r="N18" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>39</v>
       </c>
@@ -11495,8 +11550,11 @@
       <c r="N19" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O19" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>31</v>
       </c>
@@ -11533,8 +11591,11 @@
       <c r="N20" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O20" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <v>28</v>
       </c>
@@ -11571,8 +11632,11 @@
       <c r="N21" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O21" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <v>48</v>
       </c>
@@ -11609,8 +11673,11 @@
       <c r="N22" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <v>49</v>
       </c>
@@ -11647,8 +11714,11 @@
       <c r="N23" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O23" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <v>27</v>
       </c>
@@ -11683,14 +11753,17 @@
         <v>4</v>
       </c>
       <c r="N24" s="3">
+        <v>3</v>
+      </c>
+      <c r="O24" s="3">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="J1:N1"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="J1:O1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
@@ -11704,10 +11777,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M7" activeCellId="1" sqref="M9:M24 M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11726,18 +11799,18 @@
     <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
@@ -11745,82 +11818,89 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="L3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <v>279</v>
       </c>
@@ -11857,8 +11937,11 @@
       <c r="N4" s="3">
         <v>232</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>130</v>
       </c>
@@ -11895,8 +11978,11 @@
       <c r="N5" s="3">
         <v>2119</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="3">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>111</v>
       </c>
@@ -11933,8 +12019,11 @@
       <c r="N6" s="3">
         <v>4083</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" s="3">
+        <v>3764</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>67</v>
       </c>
@@ -11971,8 +12060,11 @@
       <c r="N7" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <v>77</v>
       </c>
@@ -12009,8 +12101,11 @@
       <c r="N8" s="3">
         <v>484</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="3">
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>78</v>
       </c>
@@ -12047,8 +12142,11 @@
       <c r="N9" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>74</v>
       </c>
@@ -12085,8 +12183,11 @@
       <c r="N10" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>45</v>
       </c>
@@ -12123,8 +12224,11 @@
       <c r="N11" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>61</v>
       </c>
@@ -12161,8 +12265,11 @@
       <c r="N12" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>96</v>
       </c>
@@ -12199,8 +12306,11 @@
       <c r="N13" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>44</v>
       </c>
@@ -12237,8 +12347,11 @@
       <c r="N14" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>60</v>
       </c>
@@ -12275,8 +12388,11 @@
       <c r="N15" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>99</v>
       </c>
@@ -12313,8 +12429,11 @@
       <c r="N16" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O16" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <v>31</v>
       </c>
@@ -12351,8 +12470,11 @@
       <c r="N17" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O17" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <v>39</v>
       </c>
@@ -12389,8 +12511,11 @@
       <c r="N18" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>27</v>
       </c>
@@ -12427,8 +12552,11 @@
       <c r="N19" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O19" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>34</v>
       </c>
@@ -12465,8 +12593,11 @@
       <c r="N20" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O20" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <v>38</v>
       </c>
@@ -12503,8 +12634,11 @@
       <c r="N21" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O21" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <v>28</v>
       </c>
@@ -12541,8 +12675,11 @@
       <c r="N22" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <v>29</v>
       </c>
@@ -12579,8 +12716,11 @@
       <c r="N23" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O23" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <v>36</v>
       </c>
@@ -12616,13 +12756,16 @@
       </c>
       <c r="N24" s="3">
         <v>2</v>
+      </c>
+      <c r="O24" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="J1:N1"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="J1:O1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
@@ -12636,10 +12779,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J2" sqref="J1:N1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12660,18 +12803,18 @@
     <col min="14" max="14" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
@@ -12679,82 +12822,89 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="L3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <v>1900</v>
       </c>
@@ -12791,8 +12941,11 @@
       <c r="N4" s="3">
         <v>7849</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="3">
+        <v>6657</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>664</v>
       </c>
@@ -12829,8 +12982,11 @@
       <c r="N5" s="3">
         <v>2345</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="3">
+        <v>2591</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>573</v>
       </c>
@@ -12867,8 +13023,11 @@
       <c r="N6" s="3">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>570</v>
       </c>
@@ -12905,8 +13064,11 @@
       <c r="N7" s="3">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <v>512</v>
       </c>
@@ -12943,8 +13105,11 @@
       <c r="N8" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="3">
+        <v>2145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>685</v>
       </c>
@@ -12981,8 +13146,11 @@
       <c r="N9" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>499</v>
       </c>
@@ -13019,8 +13187,11 @@
       <c r="N10" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>501</v>
       </c>
@@ -13057,8 +13228,11 @@
       <c r="N11" s="3">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>610</v>
       </c>
@@ -13095,8 +13269,11 @@
       <c r="N12" s="3">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>506</v>
       </c>
@@ -13133,8 +13310,11 @@
       <c r="N13" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>608</v>
       </c>
@@ -13171,8 +13351,11 @@
       <c r="N14" s="3">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>629</v>
       </c>
@@ -13209,8 +13392,11 @@
       <c r="N15" s="3">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>501</v>
       </c>
@@ -13247,8 +13433,11 @@
       <c r="N16" s="3">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O16" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <v>501</v>
       </c>
@@ -13285,8 +13474,11 @@
       <c r="N17" s="3">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O17" s="3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <v>573</v>
       </c>
@@ -13323,8 +13515,11 @@
       <c r="N18" s="3">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>526</v>
       </c>
@@ -13361,8 +13556,11 @@
       <c r="N19" s="3">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O19" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>512</v>
       </c>
@@ -13399,8 +13597,11 @@
       <c r="N20" s="3">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O20" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <v>578</v>
       </c>
@@ -13437,8 +13638,11 @@
       <c r="N21" s="3">
         <v>201</v>
       </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O21" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <v>1617</v>
       </c>
@@ -13475,8 +13679,11 @@
       <c r="N22" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <v>490</v>
       </c>
@@ -13513,8 +13720,11 @@
       <c r="N23" s="3">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O23" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <v>489</v>
       </c>
@@ -13550,18 +13760,21 @@
       </c>
       <c r="N24" s="3">
         <v>33</v>
+      </c>
+      <c r="O24" s="3">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="J1:N1"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -13570,10 +13783,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="R47" sqref="R47"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13584,18 +13797,18 @@
     <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
@@ -13603,352 +13816,422 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="L3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="4"/>
+      <c r="N3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="5"/>
       <c r="M4" s="3">
         <v>7715</v>
       </c>
       <c r="N4" s="3">
         <v>8316</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="4"/>
+      <c r="O4" s="3">
+        <v>7691</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="5"/>
       <c r="M5" s="3">
         <v>2113</v>
       </c>
       <c r="N5" s="3">
         <v>2153</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="4"/>
+      <c r="O5" s="3">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="5"/>
       <c r="M6" s="3">
         <v>284</v>
       </c>
       <c r="N6" s="3">
         <v>213</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="4"/>
+      <c r="O6" s="3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="5"/>
       <c r="M7" s="3">
         <v>358</v>
       </c>
       <c r="N7" s="3">
         <v>277</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="4"/>
+      <c r="O7" s="3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="5"/>
       <c r="M8" s="3">
         <v>224</v>
       </c>
       <c r="N8" s="3">
         <v>214</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="4"/>
+      <c r="O8" s="3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="5"/>
       <c r="M9" s="3">
         <v>220</v>
       </c>
       <c r="N9" s="3">
         <v>376</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="4"/>
+      <c r="O9" s="3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="5"/>
       <c r="M10" s="3">
         <v>368</v>
       </c>
       <c r="N10" s="3">
         <v>461</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="4"/>
+      <c r="O10" s="3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="5"/>
       <c r="M11" s="3">
         <v>219</v>
       </c>
       <c r="N11" s="3">
         <v>398</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="4"/>
+      <c r="O11" s="3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="5"/>
       <c r="M12" s="3">
         <v>225</v>
       </c>
       <c r="N12" s="3">
         <v>226</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="4"/>
+      <c r="O12" s="3">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="5"/>
       <c r="M13" s="3">
         <v>482</v>
       </c>
       <c r="N13" s="3">
         <v>212</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="4"/>
+      <c r="O13" s="3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="5"/>
       <c r="M14" s="3">
         <v>294</v>
       </c>
       <c r="N14" s="3">
         <v>1948</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="4"/>
+      <c r="O14" s="3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="5"/>
       <c r="M15" s="3">
         <v>263</v>
       </c>
       <c r="N15" s="3">
         <v>227</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="4"/>
+      <c r="O15" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="5"/>
       <c r="M16" s="3">
         <v>2288</v>
       </c>
       <c r="N16" s="3">
         <v>231</v>
       </c>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="4"/>
+      <c r="O16" s="3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="5"/>
       <c r="M17" s="3">
         <v>228</v>
       </c>
       <c r="N17" s="3">
         <v>400</v>
       </c>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="4"/>
+      <c r="O17" s="3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="5"/>
       <c r="M18" s="3">
         <v>222</v>
       </c>
       <c r="N18" s="3">
         <v>220</v>
       </c>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="4"/>
+      <c r="O18" s="3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="5"/>
       <c r="M19" s="3">
         <v>295</v>
       </c>
       <c r="N19" s="3">
         <v>216</v>
       </c>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="4"/>
+      <c r="O19" s="3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="5"/>
       <c r="M20" s="3">
         <v>584</v>
       </c>
       <c r="N20" s="3">
         <v>615</v>
       </c>
-    </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="4"/>
+      <c r="O20" s="3">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="5"/>
       <c r="M21" s="3">
         <v>224</v>
       </c>
       <c r="N21" s="3">
         <v>219</v>
       </c>
-    </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="4"/>
+      <c r="O21" s="3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="5"/>
       <c r="M22" s="3">
         <v>226</v>
       </c>
       <c r="N22" s="3">
         <v>231</v>
       </c>
-    </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="4"/>
+      <c r="O22" s="3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="5"/>
       <c r="M23" s="3">
         <v>221</v>
       </c>
       <c r="N23" s="3">
         <v>216</v>
       </c>
-    </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="4"/>
+      <c r="O23" s="3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="5"/>
       <c r="M24" s="3">
         <v>550</v>
       </c>
       <c r="N24" s="3">
         <v>558</v>
+      </c>
+      <c r="O24" s="3">
+        <v>610</v>
       </c>
     </row>
   </sheetData>
@@ -13956,13 +14239,332 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J1:N1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="J1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J4" s="3">
+        <v>1726</v>
+      </c>
+      <c r="P4" s="3">
+        <v>13608</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J5" s="3">
+        <v>1122</v>
+      </c>
+      <c r="P5" s="3">
+        <v>7197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J6" s="3">
+        <v>1132</v>
+      </c>
+      <c r="P6" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J7" s="3">
+        <v>992</v>
+      </c>
+      <c r="P7" s="3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J8" s="3">
+        <v>1103</v>
+      </c>
+      <c r="P8" s="3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J9" s="3">
+        <v>1001</v>
+      </c>
+      <c r="P9" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J10" s="3">
+        <v>988</v>
+      </c>
+      <c r="P10" s="3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J11" s="3">
+        <v>968</v>
+      </c>
+      <c r="P11" s="3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J12" s="3">
+        <v>1107</v>
+      </c>
+      <c r="P12" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J13" s="3">
+        <v>962</v>
+      </c>
+      <c r="P13" s="3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J14" s="3">
+        <v>1135</v>
+      </c>
+      <c r="P14" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J15" s="3">
+        <v>969</v>
+      </c>
+      <c r="P15" s="3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J16" s="3">
+        <v>1033</v>
+      </c>
+      <c r="P16" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="J17" s="3">
+        <v>1042</v>
+      </c>
+      <c r="P17" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="J18" s="3">
+        <v>1049</v>
+      </c>
+      <c r="P18" s="3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="J19" s="3">
+        <v>958</v>
+      </c>
+      <c r="P19" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="J20" s="3">
+        <v>945</v>
+      </c>
+      <c r="P20" s="3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="J21" s="3">
+        <v>1137</v>
+      </c>
+      <c r="P21" s="3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="J22" s="3">
+        <v>971</v>
+      </c>
+      <c r="P22" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="J23" s="3">
+        <v>989</v>
+      </c>
+      <c r="P23" s="3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="J24" s="3">
+        <v>935</v>
+      </c>
+      <c r="P24" s="3">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="B1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Make time measurement completely native to be able to handle longs instead of ints
</commit_message>
<xml_diff>
--- a/org.metaborg.lang.tiger.example/microbenchmarks/timings.xlsx
+++ b/org.metaborg.lang.tiger.example/microbenchmarks/timings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="32740" windowHeight="20540" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="32740" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="queens-looped" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="16">
   <si>
     <t>Iteration</t>
   </si>
@@ -80,7 +80,7 @@
     <t>5353df0622f -- RuleChains</t>
   </si>
   <si>
-    <t>5353df0622f -- FatChain</t>
+    <t>cccf26612 -- Usability tuneups</t>
   </si>
 </sst>
 </file>
@@ -167,7 +167,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,10 +178,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -908,11 +911,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1608618416"/>
-        <c:axId val="-1680217936"/>
+        <c:axId val="-2131094752"/>
+        <c:axId val="-2131092432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1608618416"/>
+        <c:axId val="-2131094752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -954,7 +957,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1680217936"/>
+        <c:crossAx val="-2131092432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -962,7 +965,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1680217936"/>
+        <c:axId val="-2131092432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300.0"/>
@@ -1014,7 +1017,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1608618416"/>
+        <c:crossAx val="-2131094752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1685,11 +1688,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1684945792"/>
-        <c:axId val="-2133179136"/>
+        <c:axId val="-2133604544"/>
+        <c:axId val="-2132927104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1684945792"/>
+        <c:axId val="-2133604544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1731,7 +1734,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133179136"/>
+        <c:crossAx val="-2132927104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1739,7 +1742,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133179136"/>
+        <c:axId val="-2132927104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -1790,7 +1793,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1684945792"/>
+        <c:crossAx val="-2133604544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2461,11 +2464,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1680595152"/>
-        <c:axId val="-1694697424"/>
+        <c:axId val="-1700247968"/>
+        <c:axId val="-1702315552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1680595152"/>
+        <c:axId val="-1700247968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2507,7 +2510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1694697424"/>
+        <c:crossAx val="-1702315552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2515,7 +2518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1694697424"/>
+        <c:axId val="-1702315552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -2566,7 +2569,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1680595152"/>
+        <c:crossAx val="-1700247968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3237,11 +3240,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2113635680"/>
-        <c:axId val="-1608873968"/>
+        <c:axId val="-1862432368"/>
+        <c:axId val="-2132554928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2113635680"/>
+        <c:axId val="-1862432368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3283,7 +3286,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1608873968"/>
+        <c:crossAx val="-2132554928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3291,7 +3294,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1608873968"/>
+        <c:axId val="-2132554928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -3342,7 +3345,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2113635680"/>
+        <c:crossAx val="-1862432368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4013,11 +4016,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1646502480"/>
-        <c:axId val="-1681822336"/>
+        <c:axId val="-1865559680"/>
+        <c:axId val="-1739440112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1646502480"/>
+        <c:axId val="-1865559680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4059,7 +4062,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1681822336"/>
+        <c:crossAx val="-1739440112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4067,7 +4070,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1681822336"/>
+        <c:axId val="-1739440112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -4118,7 +4121,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1646502480"/>
+        <c:crossAx val="-1865559680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4706,11 +4709,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1649124224"/>
-        <c:axId val="-1646090368"/>
+        <c:axId val="-2133234912"/>
+        <c:axId val="-2133232864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1649124224"/>
+        <c:axId val="-2133234912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4752,7 +4755,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1646090368"/>
+        <c:crossAx val="-2133232864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4760,7 +4763,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1646090368"/>
+        <c:axId val="-2133232864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000.0"/>
@@ -4811,7 +4814,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1649124224"/>
+        <c:crossAx val="-2133234912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8703,8 +8706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M5:M24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8718,59 +8721,60 @@
     <col min="12" max="12" width="18.5" customWidth="1"/>
     <col min="13" max="13" width="15.33203125" customWidth="1"/>
     <col min="14" max="14" width="22" customWidth="1"/>
-    <col min="15" max="16" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="2" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="8"/>
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="7"/>
       <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
@@ -9770,10 +9774,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O24" sqref="O6:O24"/>
+      <selection sqref="A1:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9795,61 +9799,64 @@
     <col min="15" max="15" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="2" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="7"/>
       <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -9895,8 +9902,11 @@
       <c r="O3" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <v>322</v>
       </c>
@@ -9937,7 +9947,7 @@
         <v>2528</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>84</v>
       </c>
@@ -9978,7 +9988,7 @@
         <v>2810</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>74</v>
       </c>
@@ -10019,7 +10029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>76</v>
       </c>
@@ -10060,7 +10070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <v>73</v>
       </c>
@@ -10101,7 +10111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>73</v>
       </c>
@@ -10142,7 +10152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>56</v>
       </c>
@@ -10183,7 +10193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>71</v>
       </c>
@@ -10224,7 +10234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>60</v>
       </c>
@@ -10265,7 +10275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>94</v>
       </c>
@@ -10306,7 +10316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>33</v>
       </c>
@@ -10347,7 +10357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>33</v>
       </c>
@@ -10388,7 +10398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>30</v>
       </c>
@@ -10775,10 +10785,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9:M24"/>
+      <selection sqref="A1:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10797,61 +10807,64 @@
     <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="2" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="7"/>
       <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -10897,8 +10910,11 @@
       <c r="O3" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <v>170</v>
       </c>
@@ -10939,7 +10955,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>124</v>
       </c>
@@ -10980,7 +10996,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>49</v>
       </c>
@@ -11021,7 +11037,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>69</v>
       </c>
@@ -11062,7 +11078,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <v>43</v>
       </c>
@@ -11103,7 +11119,7 @@
         <v>5002</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>57</v>
       </c>
@@ -11144,7 +11160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>31</v>
       </c>
@@ -11185,7 +11201,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>40</v>
       </c>
@@ -11226,7 +11242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>41</v>
       </c>
@@ -11267,7 +11283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>48</v>
       </c>
@@ -11308,7 +11324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>49</v>
       </c>
@@ -11349,7 +11365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>56</v>
       </c>
@@ -11390,7 +11406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>32</v>
       </c>
@@ -11777,10 +11793,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M7" activeCellId="1" sqref="M9:M24 M7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11799,61 +11815,64 @@
     <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="2" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="7"/>
       <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -11899,8 +11918,11 @@
       <c r="O3" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <v>279</v>
       </c>
@@ -11941,7 +11963,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>130</v>
       </c>
@@ -11982,7 +12004,7 @@
         <v>1923</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>111</v>
       </c>
@@ -12023,7 +12045,7 @@
         <v>3764</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>67</v>
       </c>
@@ -12064,7 +12086,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <v>77</v>
       </c>
@@ -12105,7 +12127,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>78</v>
       </c>
@@ -12146,7 +12168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>74</v>
       </c>
@@ -12187,7 +12209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>45</v>
       </c>
@@ -12228,7 +12250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>61</v>
       </c>
@@ -12269,7 +12291,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>96</v>
       </c>
@@ -12310,7 +12332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>44</v>
       </c>
@@ -12351,7 +12373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>60</v>
       </c>
@@ -12392,7 +12414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>99</v>
       </c>
@@ -12779,10 +12801,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection sqref="A1:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12803,61 +12825,64 @@
     <col min="14" max="14" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="2" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="7"/>
       <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -12903,8 +12928,11 @@
       <c r="O3" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <v>1900</v>
       </c>
@@ -12945,7 +12973,7 @@
         <v>6657</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>664</v>
       </c>
@@ -12986,7 +13014,7 @@
         <v>2591</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>573</v>
       </c>
@@ -13027,7 +13055,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>570</v>
       </c>
@@ -13068,7 +13096,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <v>512</v>
       </c>
@@ -13109,7 +13137,7 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>685</v>
       </c>
@@ -13150,7 +13178,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>499</v>
       </c>
@@ -13191,7 +13219,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>501</v>
       </c>
@@ -13232,7 +13260,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>610</v>
       </c>
@@ -13273,7 +13301,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>506</v>
       </c>
@@ -13314,7 +13342,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>608</v>
       </c>
@@ -13355,7 +13383,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>629</v>
       </c>
@@ -13396,7 +13424,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>501</v>
       </c>
@@ -13767,14 +13795,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J1:O1"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -13783,7 +13811,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:P3"/>
@@ -13797,61 +13825,64 @@
     <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="2" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="7"/>
       <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -13897,12 +13928,15 @@
       <c r="O3" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="P3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="5"/>
       <c r="M4" s="3">
         <v>7715</v>
@@ -13914,11 +13948,11 @@
         <v>7691</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="5"/>
       <c r="M5" s="3">
         <v>2113</v>
@@ -13930,11 +13964,11 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="5"/>
       <c r="M6" s="3">
         <v>284</v>
@@ -13946,11 +13980,11 @@
         <v>367</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="5"/>
       <c r="M7" s="3">
         <v>358</v>
@@ -13962,11 +13996,11 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="5"/>
       <c r="M8" s="3">
         <v>224</v>
@@ -13978,11 +14012,11 @@
         <v>322</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="5"/>
       <c r="M9" s="3">
         <v>220</v>
@@ -13994,11 +14028,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
       <c r="G10" s="5"/>
       <c r="M10" s="3">
         <v>368</v>
@@ -14010,11 +14044,11 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="5"/>
       <c r="M11" s="3">
         <v>219</v>
@@ -14026,11 +14060,11 @@
         <v>227</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="5"/>
       <c r="M12" s="3">
         <v>225</v>
@@ -14042,11 +14076,11 @@
         <v>466</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="5"/>
       <c r="M13" s="3">
         <v>482</v>
@@ -14058,11 +14092,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="5"/>
       <c r="M14" s="3">
         <v>294</v>
@@ -14074,11 +14108,11 @@
         <v>290</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="5"/>
       <c r="M15" s="3">
         <v>263</v>
@@ -14090,11 +14124,11 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="5"/>
       <c r="M16" s="3">
         <v>2288</v>
@@ -14107,10 +14141,10 @@
       </c>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="5"/>
       <c r="M17" s="3">
         <v>228</v>
@@ -14123,10 +14157,10 @@
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="5"/>
       <c r="M18" s="3">
         <v>222</v>
@@ -14139,10 +14173,10 @@
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="5"/>
       <c r="M19" s="3">
         <v>295</v>
@@ -14155,10 +14189,10 @@
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
       <c r="G20" s="5"/>
       <c r="M20" s="3">
         <v>584</v>
@@ -14171,10 +14205,10 @@
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
       <c r="G21" s="5"/>
       <c r="M21" s="3">
         <v>224</v>
@@ -14187,10 +14221,10 @@
       </c>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
       <c r="G22" s="5"/>
       <c r="M22" s="3">
         <v>226</v>
@@ -14203,10 +14237,10 @@
       </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
       <c r="G23" s="5"/>
       <c r="M23" s="3">
         <v>221</v>
@@ -14219,10 +14253,10 @@
       </c>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
       <c r="G24" s="5"/>
       <c r="M24" s="3">
         <v>550</v>
@@ -14236,14 +14270,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="J1:O1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="J1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14254,8 +14288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14269,71 +14303,68 @@
     <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="2" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="2"/>
       <c r="P2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -14365,22 +14396,22 @@
         <v>2</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>13</v>
@@ -14556,14 +14587,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="K1:P1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>